<commit_message>
test from silver PC
</commit_message>
<xml_diff>
--- a/Speed chart.xlsx
+++ b/Speed chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark.Balla\Projects\~FRC\GIT\2024SwerveDrive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mball\Documents\2024SwerveDrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80131FC5-D4DC-4276-9B04-37F53A4A23D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916BCAB8-2E09-4858-8CBB-ADFC52C5E433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="21599" windowHeight="11332" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -152,7 +152,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -258,7 +258,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -400,7 +400,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -414,19 +414,19 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="10" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -446,7 +446,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -480,7 +480,7 @@
         <v>4039.5</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.9</v>
       </c>
@@ -521,7 +521,7 @@
         <v>3642.5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.8</v>
       </c>
@@ -562,7 +562,7 @@
         <v>3262.5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.7</v>
       </c>
@@ -603,7 +603,7 @@
         <v>2828.5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -644,7 +644,7 @@
         <v>2376.5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.5</v>
       </c>
@@ -685,7 +685,7 @@
         <v>1922.5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.4</v>
       </c>
@@ -726,7 +726,7 @@
         <v>1422.5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.3</v>
       </c>
@@ -768,7 +768,7 @@
         <v>976.5</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.2</v>
       </c>
@@ -810,7 +810,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.1</v>
       </c>
@@ -838,59 +838,59 @@
         <v>2.8050490883590464E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>-0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>-0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>-0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>-0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>-0.7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>-0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>-0.9</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>99999</v>
+        <v>77777</v>
       </c>
       <c r="B23">
         <v>-5880</v>

</xml_diff>

<commit_message>
test silver pc push
</commit_message>
<xml_diff>
--- a/Speed chart.xlsx
+++ b/Speed chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mball\Documents\2024SwerveDrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916BCAB8-2E09-4858-8CBB-ADFC52C5E433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9517B7-47F7-4085-BC69-47A168187B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -890,7 +890,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>77777</v>
+        <v>5656565</v>
       </c>
       <c r="B23">
         <v>-5880</v>

</xml_diff>